<commit_message>
adding years won to maps
</commit_message>
<xml_diff>
--- a/FIFA_win_map/static/Project2/fifa_wins.xlsx
+++ b/FIFA_win_map/static/Project2/fifa_wins.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fractals\Desktop\UCB_analytics\GitHub\Project3_TeamX\static\Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fractals\Desktop\UCB_analytics\GitHub\Project3_TeamX\A-Team\FIFA_win_map\static\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D0F5AA4B-C728-4A7C-87BC-95F8F61DB233}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8B230B4B-8B04-4D3C-8EFE-BD8196C4506F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="6456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Wins</t>
   </si>
@@ -74,6 +74,24 @@
   </si>
   <si>
     <t>Lon</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>1958, 1962, 1970, 1994, 2002</t>
+  </si>
+  <si>
+    <t>1954, 1974, 1990, 2014</t>
+  </si>
+  <si>
+    <t>1934, 1938, 1982,  2006</t>
+  </si>
+  <si>
+    <t>1978, 1986</t>
+  </si>
+  <si>
+    <t>1930, 1950</t>
   </si>
 </sst>
 </file>
@@ -914,15 +932,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -941,8 +959,11 @@
       <c r="F1" t="s">
         <v>17</v>
       </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -961,8 +982,11 @@
       <c r="F2">
         <v>-51.9253</v>
       </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -981,8 +1005,11 @@
       <c r="F3">
         <v>10.451499999999999</v>
       </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1001,8 +1028,11 @@
       <c r="F4">
         <v>12.567399999999999</v>
       </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1021,8 +1051,11 @@
       <c r="F5">
         <v>-63.616700000000002</v>
       </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1041,8 +1074,11 @@
       <c r="F6">
         <v>-55.765799999999999</v>
       </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1061,8 +1097,11 @@
       <c r="F7">
         <v>2.2136999999999998</v>
       </c>
+      <c r="G7">
+        <v>1998</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1081,8 +1120,11 @@
       <c r="F8">
         <v>0.1278</v>
       </c>
+      <c r="G8">
+        <v>1966</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1101,8 +1143,11 @@
       <c r="F9">
         <v>-2.7492000000000001</v>
       </c>
+      <c r="G9">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1122,7 +1167,7 @@
         <v>5.2912999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1142,7 +1187,7 @@
         <v>15.473000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1162,7 +1207,7 @@
         <v>19.503299999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>

</xml_diff>